<commit_message>
Scrapers adaptados a nuevo contexto
</commit_message>
<xml_diff>
--- a/db/data.xlsx
+++ b/db/data.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrei.flores\Documents\Trabajo\Scraping-Tendencias\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C165C68C-5A59-466C-9707-3E9F51B9B143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6534666C-93E5-4693-9643-40485B730D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Carreras" sheetId="1" r:id="rId1"/>
     <sheet name="Codigos" sheetId="9" state="hidden" r:id="rId2"/>
-    <sheet name="Semrush" sheetId="11" state="hidden" r:id="rId3"/>
-    <sheet name="SemrushBase" sheetId="7" state="hidden" r:id="rId4"/>
-    <sheet name="GoogleTrendsBase" sheetId="8" state="hidden" r:id="rId5"/>
-    <sheet name="Input" sheetId="10" r:id="rId6"/>
-    <sheet name="LinkedIn" sheetId="5" state="hidden" r:id="rId7"/>
+    <sheet name="SemrushBase" sheetId="7" r:id="rId3"/>
+    <sheet name="GoogleTrendsBase" sheetId="8" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="337">
   <si>
     <t>Facultad</t>
   </si>
@@ -128,15 +125,6 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t>Total Ingresos</t>
-  </si>
-  <si>
-    <t>Ventas 12%</t>
-  </si>
-  <si>
-    <t>Ventas 0%</t>
-  </si>
-  <si>
     <t>Visión General</t>
   </si>
   <si>
@@ -512,51 +500,9 @@
     <t>Codigo</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Profesionales</t>
-  </si>
-  <si>
-    <t>Anuncios de empleo</t>
-  </si>
-  <si>
-    <t>Demanda de contratacion</t>
-  </si>
-  <si>
-    <t>%Anuncios/Profesionales</t>
-  </si>
-  <si>
     <t>O8421.01</t>
   </si>
   <si>
-    <t>LINKEDIN</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Proyecto</t>
-  </si>
-  <si>
-    <t>Carpeta</t>
-  </si>
-  <si>
-    <t>Referencia</t>
-  </si>
-  <si>
-    <t>Consulta</t>
-  </si>
-  <si>
-    <t>SEMRUSH</t>
-  </si>
-  <si>
-    <t>CARRERA</t>
-  </si>
-  <si>
-    <t>MERCADO</t>
-  </si>
-  <si>
     <t>J620101</t>
   </si>
   <si>
@@ -695,85 +641,415 @@
     <t>C182001</t>
   </si>
   <si>
-    <t>OFERTA</t>
-  </si>
-  <si>
-    <t>Virtualidad</t>
-  </si>
-  <si>
-    <t>Presencialidad</t>
-  </si>
-  <si>
-    <t>TRENDS</t>
-  </si>
-  <si>
-    <t>Negocios Deportivos</t>
-  </si>
-  <si>
-    <t>Gestión deportiva</t>
-  </si>
-  <si>
-    <t>1,88</t>
-  </si>
-  <si>
-    <t>Marketing Deportivo</t>
-  </si>
-  <si>
-    <t>Eventos</t>
-  </si>
-  <si>
-    <t>8,26</t>
-  </si>
-  <si>
-    <t>Patrocinio</t>
-  </si>
-  <si>
-    <t>50,2</t>
-  </si>
-  <si>
-    <t>Innovación</t>
-  </si>
-  <si>
-    <t>26,5</t>
-  </si>
-  <si>
-    <t>Comunicación en el deporte</t>
-  </si>
-  <si>
-    <t>Futbol</t>
-  </si>
-  <si>
-    <t>49,8</t>
-  </si>
-  <si>
-    <t>Deporte</t>
-  </si>
-  <si>
-    <t>20,6</t>
-  </si>
-  <si>
-    <t>Maestría en Dirección de Negocios Deportivos e Innovación</t>
-  </si>
-  <si>
-    <t>MAESTRIA DIRECCION NEGOCIOS DEPORTIVOS</t>
-  </si>
-  <si>
-    <t>POSGRADOS TENDENCIA</t>
-  </si>
-  <si>
-    <t>Ecuador</t>
-  </si>
-  <si>
-    <t>Baja</t>
-  </si>
-  <si>
-    <t>América Latina</t>
-  </si>
-  <si>
-    <t>MAESTRIA EN GESTION DEL TALENTO HUMANO MENCION DESARROLLO ORGANIZACIONAL</t>
-  </si>
-  <si>
-    <t>Moderada</t>
+    <t>Nivel</t>
+  </si>
+  <si>
+    <t>Pregrado</t>
+  </si>
+  <si>
+    <t>Posgrado</t>
+  </si>
+  <si>
+    <t>Maestria en gerencia politica, gobernanza y gobernabilidad</t>
+  </si>
+  <si>
+    <t>Escuela de negocios</t>
+  </si>
+  <si>
+    <t>Maestria en administracion de empresas mba</t>
+  </si>
+  <si>
+    <t>Maestria en psicoterapia</t>
+  </si>
+  <si>
+    <t>Maestria en diseño arquitectonico avanzado</t>
+  </si>
+  <si>
+    <t>Maestria en direccion y postproduccion audiovisual</t>
+  </si>
+  <si>
+    <t>Maestria en derecho procesal constitucional</t>
+  </si>
+  <si>
+    <t>Maestria en transformacion digital y gestion de la innovacion</t>
+  </si>
+  <si>
+    <t>Especialidad en ortodoncia</t>
+  </si>
+  <si>
+    <t>Maestria en neuromarketing</t>
+  </si>
+  <si>
+    <t>Maestria en enfermeria</t>
+  </si>
+  <si>
+    <t>Liderazgo político</t>
+  </si>
+  <si>
+    <t>Políticas públicas</t>
+  </si>
+  <si>
+    <t>Gestión pública</t>
+  </si>
+  <si>
+    <t>Gobernanza digital</t>
+  </si>
+  <si>
+    <t>Transparencia institucional</t>
+  </si>
+  <si>
+    <t>Participación ciudadana</t>
+  </si>
+  <si>
+    <t>Innovación educativa</t>
+  </si>
+  <si>
+    <t>Transformación digital</t>
+  </si>
+  <si>
+    <t>Análisis político</t>
+  </si>
+  <si>
+    <t>Desarrollo sostenible</t>
+  </si>
+  <si>
+    <t>Liderazgo</t>
+  </si>
+  <si>
+    <t>Gestión</t>
+  </si>
+  <si>
+    <t>Administración</t>
+  </si>
+  <si>
+    <t>Analisis de datos</t>
+  </si>
+  <si>
+    <t>Empresas</t>
+  </si>
+  <si>
+    <t>Emprendimiento</t>
+  </si>
+  <si>
+    <t>Sostenibilidad</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Finanzas corporativas</t>
+  </si>
+  <si>
+    <t>Directiva</t>
+  </si>
+  <si>
+    <t>Salud mental</t>
+  </si>
+  <si>
+    <t>Terapia cognitiva</t>
+  </si>
+  <si>
+    <t>Mindfulness laboral</t>
+  </si>
+  <si>
+    <t>Neurociencia aplicada</t>
+  </si>
+  <si>
+    <t>Inteligencia emocional</t>
+  </si>
+  <si>
+    <t>Psicología positiva</t>
+  </si>
+  <si>
+    <t>Terapia virtual</t>
+  </si>
+  <si>
+    <t>Compasión terapéutica</t>
+  </si>
+  <si>
+    <t>Psicoterapia integral</t>
+  </si>
+  <si>
+    <t>Diseño sostenible</t>
+  </si>
+  <si>
+    <t>Realidad virtual</t>
+  </si>
+  <si>
+    <t>Arquitectura modular</t>
+  </si>
+  <si>
+    <t>Diseño paramétrico</t>
+  </si>
+  <si>
+    <t>BIM</t>
+  </si>
+  <si>
+    <t>Impresión 3D</t>
+  </si>
+  <si>
+    <t>Diseño biofílico</t>
+  </si>
+  <si>
+    <t>Espacios flexibles</t>
+  </si>
+  <si>
+    <t>Arquitectura resiliente</t>
+  </si>
+  <si>
+    <t>Diseño inclusivo</t>
+  </si>
+  <si>
+    <t>Cuidados intensivos</t>
+  </si>
+  <si>
+    <t>Enfermeria</t>
+  </si>
+  <si>
+    <t>Gestión hospitalaria</t>
+  </si>
+  <si>
+    <t>Educación continua</t>
+  </si>
+  <si>
+    <t>Simulación clínica</t>
+  </si>
+  <si>
+    <t>Atención primaria</t>
+  </si>
+  <si>
+    <t>Enfermería avanzada</t>
+  </si>
+  <si>
+    <t>Liderazgo clínico</t>
+  </si>
+  <si>
+    <t>Neuromarketing</t>
+  </si>
+  <si>
+    <t>Neuroventas</t>
+  </si>
+  <si>
+    <t>Análisis emocional</t>
+  </si>
+  <si>
+    <t>Inteligencia artificial</t>
+  </si>
+  <si>
+    <t>Realidad aumentada</t>
+  </si>
+  <si>
+    <t>Big data</t>
+  </si>
+  <si>
+    <t>Experiencia de usuario</t>
+  </si>
+  <si>
+    <t>Marketing sensorial</t>
+  </si>
+  <si>
+    <t>Comportamiento del consumidor</t>
+  </si>
+  <si>
+    <t>Postproducción digital</t>
+  </si>
+  <si>
+    <t>Dirección audiovisual</t>
+  </si>
+  <si>
+    <t>Colorización avanzada</t>
+  </si>
+  <si>
+    <t>Montaje cinematográfico</t>
+  </si>
+  <si>
+    <t>Narrativa transmedia</t>
+  </si>
+  <si>
+    <t>Producción virtual</t>
+  </si>
+  <si>
+    <t>Animación 3D</t>
+  </si>
+  <si>
+    <t>Edición colaborativa</t>
+  </si>
+  <si>
+    <t>Litigación constitucional</t>
+  </si>
+  <si>
+    <t>Derecho procesal</t>
+  </si>
+  <si>
+    <t>Control de constitucionalidad</t>
+  </si>
+  <si>
+    <t>Derechos fundamentales</t>
+  </si>
+  <si>
+    <t>Justicia constitucional</t>
+  </si>
+  <si>
+    <t>Garantías jurisdiccionales</t>
+  </si>
+  <si>
+    <t>Interpretación constitucional</t>
+  </si>
+  <si>
+    <t>Derecho comparado</t>
+  </si>
+  <si>
+    <t>Acción de protección</t>
+  </si>
+  <si>
+    <t>Derecho constitucional</t>
+  </si>
+  <si>
+    <t>Director de Transformación Digital</t>
+  </si>
+  <si>
+    <t>Gerente de Innovación</t>
+  </si>
+  <si>
+    <t>Consultor en Transformación Digital</t>
+  </si>
+  <si>
+    <t>Gerente de Proyectos de Innovación</t>
+  </si>
+  <si>
+    <t>Estratega de Innovación Empresarial</t>
+  </si>
+  <si>
+    <t>Analista de Datos</t>
+  </si>
+  <si>
+    <t>Especialista en Ciberseguridad</t>
+  </si>
+  <si>
+    <t>Emprendedor en Startups Tecnológicas</t>
+  </si>
+  <si>
+    <t>Marketing Digital</t>
+  </si>
+  <si>
+    <t>Investigador</t>
+  </si>
+  <si>
+    <t>Brackets estéticos</t>
+  </si>
+  <si>
+    <t>Ortodoncia lingual</t>
+  </si>
+  <si>
+    <t>Alineadores transparentes</t>
+  </si>
+  <si>
+    <t>Ortodoncia digital</t>
+  </si>
+  <si>
+    <t>Ortodoncia interceptiva</t>
+  </si>
+  <si>
+    <t>Maloclusión dental</t>
+  </si>
+  <si>
+    <t>Diagnóstico 3D</t>
+  </si>
+  <si>
+    <t>Ortodoncia infantil</t>
+  </si>
+  <si>
+    <t>Técnicas avanzadas</t>
+  </si>
+  <si>
+    <t>O841101</t>
+  </si>
+  <si>
+    <t>O841102</t>
+  </si>
+  <si>
+    <t>O841103</t>
+  </si>
+  <si>
+    <t>O841104</t>
+  </si>
+  <si>
+    <t>O841105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O841106 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M701000  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M702001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M702002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M702003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q872002  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q872003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M711021  </t>
+  </si>
+  <si>
+    <t>M711022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M711012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q869011 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q871003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M731004 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M731002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M731003 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M731001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J591201 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J591100 </t>
+  </si>
+  <si>
+    <t>M691001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M691002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M691009 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J620210 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J631101  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q862002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q862004 </t>
   </si>
 </sst>
 </file>
@@ -797,56 +1073,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -861,55 +1099,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -927,6 +1125,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -960,10 +1161,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93318B00-F1FB-40E0-A852-3B604D247CB6}" name="carreras" displayName="carreras" ref="A1:C13" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:C13" xr:uid="{93318B00-F1FB-40E0-A852-3B604D247CB6}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93318B00-F1FB-40E0-A852-3B604D247CB6}" name="carreras" displayName="carreras" ref="A1:D23" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:D23" xr:uid="{93318B00-F1FB-40E0-A852-3B604D247CB6}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A8A8B14F-B664-4097-BE16-5A8099D1D2FD}" name="Facultad"/>
+    <tableColumn id="4" xr3:uid="{80078F35-C3FE-43CF-9E83-31878256DD08}" name="Nivel"/>
     <tableColumn id="2" xr3:uid="{90ADE1FE-7EB4-4B5B-9DBB-D53357149D2D}" name="Carrera"/>
     <tableColumn id="3" xr3:uid="{60374FED-47F6-4CAB-BE1F-C2BE8A72D5D4}" name="ID"/>
   </tableColumns>
@@ -971,46 +1173,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E222F82A-B1CE-4CB1-B3D5-F5F03CB778BB}" name="ofertaCarrera" displayName="ofertaCarrera" ref="O4:P5" totalsRowShown="0">
-  <autoFilter ref="O4:P5" xr:uid="{E222F82A-B1CE-4CB1-B3D5-F5F03CB778BB}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{53DF69A2-9BF8-48DB-A48E-80DBFCC3B273}" name="Virtualidad"/>
-    <tableColumn id="2" xr3:uid="{64CE4ECA-AEE4-4B82-B9F4-6346F6D39658}" name="Presencialidad"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{FF2B5D86-C5C0-484E-A4C7-3A05286345F5}" name="palabrasTrends" displayName="palabrasTrends" ref="H4:I14" totalsRowShown="0">
-  <autoFilter ref="H4:I14" xr:uid="{FF2B5D86-C5C0-484E-A4C7-3A05286345F5}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9693F56C-EFFD-4B3B-A80A-DC6F04CFB8D4}" name="Palabras"/>
-    <tableColumn id="2" xr3:uid="{BE181839-C9A5-4B63-9DF9-A37F23208C42}" name="Cantidad" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{583667FE-FA14-497A-A7F6-8A2926B2693C}" name="datoLinkedin" displayName="datoLinkedin" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5" xr:uid="{583667FE-FA14-497A-A7F6-8A2926B2693C}"/>
-  <tableColumns count="6">
-    <tableColumn id="8" xr3:uid="{1355639F-4CD3-496D-9612-6BD9CA9C1B7B}" name="Tipo"/>
-    <tableColumn id="1" xr3:uid="{C2B4260C-0176-46CE-9F8F-832065A82854}" name="Region"/>
-    <tableColumn id="2" xr3:uid="{4DFFDF20-F4C9-41FF-944B-701927076702}" name="Profesionales"/>
-    <tableColumn id="3" xr3:uid="{810277DA-2B5E-4CF9-842D-38212D329437}" name="Anuncios de empleo"/>
-    <tableColumn id="4" xr3:uid="{9CF7AEF5-F450-4386-A537-31F9ACF58C69}" name="%Anuncios/Profesionales"/>
-    <tableColumn id="5" xr3:uid="{10DB73B1-B884-4D95-B9B3-4BF97DE7C6A6}" name="Demanda de contratacion"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{68803FB0-62D8-4DB7-A858-582C7C641EAB}" name="codigosCarreras" displayName="codigosCarreras" ref="A1:B52" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:B52" xr:uid="{68803FB0-62D8-4DB7-A858-582C7C641EAB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{68803FB0-62D8-4DB7-A858-582C7C641EAB}" name="codigosCarreras" displayName="codigosCarreras" ref="A1:B87" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B87" xr:uid="{68803FB0-62D8-4DB7-A858-582C7C641EAB}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{06E615E8-0A2E-4DB9-948C-4A44CF99AC22}" name="ID Carrera"/>
     <tableColumn id="2" xr3:uid="{83C244AF-FCAA-4DD0-A8A8-092D3787DDB3}" name="Codigo"/>
@@ -1020,20 +1185,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{26CBC741-88AF-4630-8543-06CABD3D7FA4}" name="datoSemrush" displayName="datoSemrush" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2" xr:uid="{81B8F745-5421-4B67-8A4F-8621CEEBF0AF}"/>
-  <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{CC0770FF-D01D-40B7-A2E2-A0EF672EAAFE}" name="Visión General"/>
-    <tableColumn id="3" xr3:uid="{B0ECF710-0C6B-4A02-A4B0-BE0973CF84F9}" name="Palabras"/>
-    <tableColumn id="4" xr3:uid="{ABA8B5AC-63CB-4A0E-AA8E-423121CDDEEB}" name="Volumen"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81B8F745-5421-4B67-8A4F-8621CEEBF0AF}" name="datoSemrushBase" displayName="datoSemrushBase" ref="A1:D13" totalsRowShown="0">
-  <autoFilter ref="A1:D13" xr:uid="{81B8F745-5421-4B67-8A4F-8621CEEBF0AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81B8F745-5421-4B67-8A4F-8621CEEBF0AF}" name="datoSemrushBase" displayName="datoSemrushBase" ref="A1:D23" totalsRowShown="0">
+  <autoFilter ref="A1:D23" xr:uid="{81B8F745-5421-4B67-8A4F-8621CEEBF0AF}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CF9B0BAD-6003-4AE9-8300-1A4BC77C59BD}" name="ID Carrera"/>
     <tableColumn id="2" xr3:uid="{A22867B5-164B-4891-AD46-C059D073B2D9}" name="Visión General"/>
@@ -1044,56 +1197,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC1640AC-A0DF-4A7A-A1E5-54F8503BBE7A}" name="palabrasTrendsBase" displayName="palabrasTrendsBase" ref="A1:C121" totalsRowShown="0">
-  <autoFilter ref="A1:C121" xr:uid="{AC1640AC-A0DF-4A7A-A1E5-54F8503BBE7A}"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC1640AC-A0DF-4A7A-A1E5-54F8503BBE7A}" name="palabrasTrendsBase" displayName="palabrasTrendsBase" ref="A1:C221" totalsRowShown="0">
+  <autoFilter ref="A1:C221" xr:uid="{AC1640AC-A0DF-4A7A-A1E5-54F8503BBE7A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2D9D27E0-D2E6-4E7B-AD1E-B9A2B24AE7D8}" name="ID Carrera"/>
     <tableColumn id="2" xr3:uid="{97E12D03-BE4B-4C2B-A771-432322741AA7}" name="Palabra"/>
-    <tableColumn id="3" xr3:uid="{B548BFA7-4463-435E-8DC9-36285EC6F069}" name="Cantidad" dataDxfId="4"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{6E4C88A0-4764-4539-B2B8-5EC705D8FD66}" name="reporteLinkedin" displayName="reporteLinkedin" ref="C4:D6" totalsRowShown="0">
-  <autoFilter ref="C4:D6" xr:uid="{6E4C88A0-4764-4539-B2B8-5EC705D8FD66}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EC17322E-C64C-434A-8EDA-48D3FD07D0D2}" name="Carpeta"/>
-    <tableColumn id="2" xr3:uid="{14383BCF-F1F9-464E-A558-7E80417C9AF8}" name="Proyecto"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{15E95354-7A2F-4C9F-BC28-D22AB3A9F1DE}" name="carreraSemrush" displayName="carreraSemrush" ref="F4:F5" totalsRowShown="0">
-  <autoFilter ref="F4:F5" xr:uid="{15E95354-7A2F-4C9F-BC28-D22AB3A9F1DE}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{DAA7970E-505B-4D8E-AB2A-9D490D17104C}" name="Consulta"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4623FD81-F3B5-44CC-9BC7-B5387944122B}" name="carreraReferencia" displayName="carreraReferencia" ref="A4:A5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="A4:A5" xr:uid="{4623FD81-F3B5-44CC-9BC7-B5387944122B}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{01035A90-4C59-4CCB-A7CB-93013B564B30}" name="Referencia" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2771B87-581B-43EB-9A03-43A23C5322C8}" name="mercado" displayName="mercado" ref="K4:M5" totalsRowShown="0">
-  <autoFilter ref="K4:M5" xr:uid="{C2771B87-581B-43EB-9A03-43A23C5322C8}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F8EE43DB-6982-4E2B-84D3-843F8B5A28C0}" name="Total Ingresos"/>
-    <tableColumn id="2" xr3:uid="{19D975BD-EFFA-4D39-9831-0AEC2D116240}" name="Ventas 12%"/>
-    <tableColumn id="3" xr3:uid="{D62ECA70-ECFB-4827-9FB9-C8A0D52AEFAB}" name="Ventas 0%"/>
+    <tableColumn id="3" xr3:uid="{B548BFA7-4463-435E-8DC9-36285EC6F069}" name="Cantidad" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1362,160 +1472,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="3" max="3" width="69" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" t="s">
+        <v>206</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C18" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" t="s">
+        <v>210</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" t="s">
+        <v>213</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1528,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1120C9F4-9471-44C8-9F5F-AFE7754F0EB2}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,10 +1831,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1552,7 +1842,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1850,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1592,7 +1882,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1600,7 +1890,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1608,7 +1898,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1616,7 +1906,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1624,7 +1914,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1632,7 +1922,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1640,7 +1930,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1648,7 +1938,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1656,7 +1946,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1664,7 +1954,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1672,7 +1962,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1680,7 +1970,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1688,7 +1978,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1696,7 +1986,7 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1704,7 +1994,7 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1712,7 +2002,7 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1720,7 +2010,7 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1728,7 +2018,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1736,7 +2026,7 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1744,7 +2034,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1752,7 +2042,7 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1760,7 +2050,7 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1768,7 +2058,7 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1776,7 +2066,7 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1784,7 +2074,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1792,7 +2082,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1800,7 +2090,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1808,7 +2098,7 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1816,7 +2106,7 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1824,7 +2114,7 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1832,7 +2122,7 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1840,7 +2130,7 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1848,7 +2138,7 @@
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1856,7 +2146,7 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1864,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1872,7 +2162,7 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1880,7 +2170,7 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1888,7 +2178,7 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1896,7 +2186,7 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1904,7 +2194,7 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1912,7 +2202,7 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1920,7 +2210,7 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1928,7 +2218,7 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1936,7 +2226,7 @@
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1944,7 +2234,7 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1952,10 +2242,291 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>197</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>13</v>
+      </c>
+      <c r="B58" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>14</v>
+      </c>
+      <c r="B59" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>14</v>
+      </c>
+      <c r="B60" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>14</v>
+      </c>
+      <c r="B62" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>15</v>
+      </c>
+      <c r="B64" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>15</v>
+      </c>
+      <c r="B65" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>22</v>
+      </c>
+      <c r="B70" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>22</v>
+      </c>
+      <c r="B71" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>22</v>
+      </c>
+      <c r="B72" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>17</v>
+      </c>
+      <c r="B73" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>17</v>
+      </c>
+      <c r="B74" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>17</v>
+      </c>
+      <c r="B75" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>17</v>
+      </c>
+      <c r="B76" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>18</v>
+      </c>
+      <c r="B77" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>18</v>
+      </c>
+      <c r="B78" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>18</v>
+      </c>
+      <c r="B79" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>19</v>
+      </c>
+      <c r="B80" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>19</v>
+      </c>
+      <c r="B81" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>19</v>
+      </c>
+      <c r="B82" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>21</v>
+      </c>
+      <c r="B86" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>21</v>
+      </c>
+      <c r="B87" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1964,54 +2535,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBF05D7-B3AC-45C8-B3E1-6C5DEAEEBA34}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C774B23-B973-484E-B73E-FF200214CF5B}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C774B23-B973-484E-B73E-FF200214CF5B}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,16 +2550,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
         <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,6 +2728,56 @@
       </c>
       <c r="D13">
         <v>1050</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2210,27 +2788,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9CF51A-F55C-43ED-BF2C-9429359FD93F}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B217" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>27</v>
@@ -2241,7 +2819,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2">
         <v>10</v>
@@ -2252,7 +2830,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2">
         <v>15.901960784313726</v>
@@ -2263,7 +2841,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>13.254901960784315</v>
@@ -2274,7 +2852,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2">
         <v>7.5490196078431371</v>
@@ -2285,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2">
         <v>56.901960784313722</v>
@@ -2296,7 +2874,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>14.941176470588236</v>
@@ -2307,7 +2885,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
         <v>15.372549019607844</v>
@@ -2318,7 +2896,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2">
         <v>30.666666666666668</v>
@@ -2329,7 +2907,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2">
         <v>8.8039215686274517</v>
@@ -2340,7 +2918,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2">
         <v>8.4313725490196081</v>
@@ -2351,7 +2929,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2">
         <v>9.0980392156862742</v>
@@ -2362,7 +2940,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2">
         <v>7.882352941176471</v>
@@ -2373,7 +2951,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2">
         <v>9.3921568627450984</v>
@@ -2384,7 +2962,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2">
         <v>8.9019607843137258</v>
@@ -2395,7 +2973,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2">
         <v>10</v>
@@ -2406,7 +2984,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2">
         <v>16</v>
@@ -2417,7 +2995,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2">
         <v>7.882352941176471</v>
@@ -2428,7 +3006,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2">
         <v>7.0392156862745097</v>
@@ -2439,7 +3017,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2">
         <v>8.3137254901960791</v>
@@ -2450,7 +3028,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2">
         <v>7.5294117647058822</v>
@@ -2461,7 +3039,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2">
         <v>9.5686274509803919</v>
@@ -2472,7 +3050,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2">
         <v>5.3725490196078427</v>
@@ -2483,7 +3061,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2">
         <v>12.568627450980401</v>
@@ -2494,7 +3072,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2">
         <v>8.2549019607843146</v>
@@ -2505,7 +3083,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2">
         <v>10.117647058823529</v>
@@ -2516,7 +3094,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2">
         <v>11.745098039215685</v>
@@ -2527,7 +3105,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C28" s="2">
         <v>9.3333333333333339</v>
@@ -2538,7 +3116,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C29" s="2">
         <v>11.784313725490197</v>
@@ -2549,7 +3127,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2">
         <v>5.8431372549019605</v>
@@ -2560,7 +3138,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C31" s="2">
         <v>8.7843137254901968</v>
@@ -2571,7 +3149,7 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C32" s="2">
         <v>10.196078431372548</v>
@@ -2582,7 +3160,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2">
         <v>6.5882352941176467</v>
@@ -2593,7 +3171,7 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C34" s="2">
         <v>10.215686274509803</v>
@@ -2604,7 +3182,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C35" s="2">
         <v>12.921568627450981</v>
@@ -2615,7 +3193,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2">
         <v>12.705882352941176</v>
@@ -2626,7 +3204,7 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C37" s="2">
         <v>14.784313725490197</v>
@@ -2637,7 +3215,7 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C38" s="2">
         <v>10.764705882352942</v>
@@ -2648,7 +3226,7 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C39" s="2">
         <v>13.019607843137255</v>
@@ -2659,7 +3237,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C40" s="2">
         <v>9.6666666666666661</v>
@@ -2670,7 +3248,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C41" s="2">
         <v>9.2549019607843146</v>
@@ -2681,7 +3259,7 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C42" s="2">
         <v>19.784313725490197</v>
@@ -2692,7 +3270,7 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C43" s="2">
         <v>11.176470588235293</v>
@@ -2703,7 +3281,7 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C44" s="2">
         <v>10.274509803921569</v>
@@ -2714,7 +3292,7 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C45" s="2">
         <v>7.8627450980392153</v>
@@ -2725,7 +3303,7 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C46" s="2">
         <v>8.1960784313725483</v>
@@ -2736,7 +3314,7 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C47" s="2">
         <v>8.2549019607843146</v>
@@ -2747,7 +3325,7 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C48" s="2">
         <v>10.294117647058824</v>
@@ -2758,7 +3336,7 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C49" s="2">
         <v>11.431372549019608</v>
@@ -2769,7 +3347,7 @@
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C50" s="2">
         <v>6.4509803921568629</v>
@@ -2780,7 +3358,7 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C51" s="2">
         <v>10.137254901960784</v>
@@ -2791,7 +3369,7 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C52" s="2">
         <v>10.176470588235293</v>
@@ -2802,7 +3380,7 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C53" s="2">
         <v>6.666666666666667</v>
@@ -2813,7 +3391,7 @@
         <v>6</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C54" s="2">
         <v>6.882352941176471</v>
@@ -2824,7 +3402,7 @@
         <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C55" s="2">
         <v>9.2156862745098032</v>
@@ -2835,7 +3413,7 @@
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C56" s="2">
         <v>12.803921568627452</v>
@@ -2846,7 +3424,7 @@
         <v>6</v>
       </c>
       <c r="B57" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C57" s="2">
         <v>9.4901960784313726</v>
@@ -2857,7 +3435,7 @@
         <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C58" s="2">
         <v>7.8039215686274508</v>
@@ -2868,7 +3446,7 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C59" s="2">
         <v>13.03921568627451</v>
@@ -2879,7 +3457,7 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C60" s="2">
         <v>15.686274509803921</v>
@@ -2890,7 +3468,7 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C61" s="2">
         <v>7.7450980392156863</v>
@@ -2901,7 +3479,7 @@
         <v>7</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C62" s="2">
         <v>11.647058823529411</v>
@@ -2912,7 +3490,7 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C63" s="2">
         <v>9.3529411764705888</v>
@@ -2923,7 +3501,7 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C64" s="2">
         <v>8.117647058823529</v>
@@ -2934,7 +3512,7 @@
         <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C65" s="2">
         <v>9.882352941176471</v>
@@ -2945,7 +3523,7 @@
         <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C66" s="2">
         <v>13.137254901960784</v>
@@ -2956,7 +3534,7 @@
         <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C67" s="2">
         <v>12.882352941176471</v>
@@ -2967,7 +3545,7 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C68" s="2">
         <v>11.607843137254902</v>
@@ -2978,7 +3556,7 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C69" s="2">
         <v>12.490196078431373</v>
@@ -2989,7 +3567,7 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C70" s="2">
         <v>15.058823529411764</v>
@@ -3000,7 +3578,7 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C71" s="2">
         <v>11.921568627450981</v>
@@ -3011,7 +3589,7 @@
         <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C72" s="2">
         <v>12.392156862745098</v>
@@ -3022,7 +3600,7 @@
         <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C73" s="2">
         <v>11.294117647058824</v>
@@ -3033,7 +3611,7 @@
         <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C74" s="2">
         <v>19.392156862745097</v>
@@ -3044,7 +3622,7 @@
         <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C75" s="2">
         <v>24.882352941176471</v>
@@ -3055,7 +3633,7 @@
         <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C76" s="2">
         <v>7.882352941176471</v>
@@ -3066,7 +3644,7 @@
         <v>8</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C77" s="2">
         <v>6.5882352941176467</v>
@@ -3077,7 +3655,7 @@
         <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C78" s="2">
         <v>11.784313725490197</v>
@@ -3088,7 +3666,7 @@
         <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C79" s="2">
         <v>8.2549019607843146</v>
@@ -3099,7 +3677,7 @@
         <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C80" s="2">
         <v>14.196078431372548</v>
@@ -3110,7 +3688,7 @@
         <v>8</v>
       </c>
       <c r="B81" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C81" s="2">
         <v>10.098039215686274</v>
@@ -3121,7 +3699,7 @@
         <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C82" s="2">
         <v>42.607843137254903</v>
@@ -3132,7 +3710,7 @@
         <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C83" s="2">
         <v>15.450980392156863</v>
@@ -3143,7 +3721,7 @@
         <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C84" s="2">
         <v>11.03921568627451</v>
@@ -3154,7 +3732,7 @@
         <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C85" s="2">
         <v>12.686274509803921</v>
@@ -3165,7 +3743,7 @@
         <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C86" s="2">
         <v>6.3137254901960782</v>
@@ -3176,7 +3754,7 @@
         <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C87" s="2">
         <v>12.196078431372548</v>
@@ -3187,7 +3765,7 @@
         <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C88" s="2">
         <v>6.882352941176471</v>
@@ -3198,7 +3776,7 @@
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C89" s="2">
         <v>6.6862745098039218</v>
@@ -3209,7 +3787,7 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C90" s="2">
         <v>13.450980392156863</v>
@@ -3220,7 +3798,7 @@
         <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C91" s="2">
         <v>5.6274509803921573</v>
@@ -3231,7 +3809,7 @@
         <v>10</v>
       </c>
       <c r="B92" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C92" s="2">
         <v>8.8039215686274517</v>
@@ -3242,7 +3820,7 @@
         <v>10</v>
       </c>
       <c r="B93" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C93" s="2">
         <v>14.666666666666666</v>
@@ -3253,7 +3831,7 @@
         <v>10</v>
       </c>
       <c r="B94" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C94" s="2">
         <v>6.9607843137254903</v>
@@ -3264,7 +3842,7 @@
         <v>10</v>
       </c>
       <c r="B95" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C95" s="2">
         <v>7.2352941176470589</v>
@@ -3275,7 +3853,7 @@
         <v>10</v>
       </c>
       <c r="B96" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C96" s="2">
         <v>7.8627450980392153</v>
@@ -3286,7 +3864,7 @@
         <v>10</v>
       </c>
       <c r="B97" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C97" s="2">
         <v>13.196078431372548</v>
@@ -3297,7 +3875,7 @@
         <v>10</v>
       </c>
       <c r="B98" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C98" s="2">
         <v>18.392156862745097</v>
@@ -3308,7 +3886,7 @@
         <v>10</v>
       </c>
       <c r="B99" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C99" s="2">
         <v>9.4313725490196081</v>
@@ -3319,7 +3897,7 @@
         <v>10</v>
       </c>
       <c r="B100" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C100" s="2">
         <v>13.470588235294118</v>
@@ -3330,7 +3908,7 @@
         <v>10</v>
       </c>
       <c r="B101" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C101" s="2">
         <v>5.3529411764705879</v>
@@ -3341,7 +3919,7 @@
         <v>11</v>
       </c>
       <c r="B102" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C102" s="2">
         <v>12.078431372549019</v>
@@ -3352,7 +3930,7 @@
         <v>11</v>
       </c>
       <c r="B103" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C103" s="2">
         <v>9.0980392156862742</v>
@@ -3363,7 +3941,7 @@
         <v>11</v>
       </c>
       <c r="B104" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C104" s="2">
         <v>8.0980392156862742</v>
@@ -3374,7 +3952,7 @@
         <v>11</v>
       </c>
       <c r="B105" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C105" s="2">
         <v>12.352941176470589</v>
@@ -3385,7 +3963,7 @@
         <v>11</v>
       </c>
       <c r="B106" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C106" s="2">
         <v>9.6470588235294112</v>
@@ -3396,7 +3974,7 @@
         <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C107" s="2">
         <v>9.6862745098039209</v>
@@ -3407,7 +3985,7 @@
         <v>11</v>
       </c>
       <c r="B108" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C108" s="2">
         <v>9.3921568627450984</v>
@@ -3418,7 +3996,7 @@
         <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C109" s="2">
         <v>8.0980392156862742</v>
@@ -3429,7 +4007,7 @@
         <v>11</v>
       </c>
       <c r="B110" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C110" s="2">
         <v>12.96078431372549</v>
@@ -3440,7 +4018,7 @@
         <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C111" s="2">
         <v>7.5098039215686274</v>
@@ -3451,7 +4029,7 @@
         <v>12</v>
       </c>
       <c r="B112" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C112" s="2">
         <v>14.96078431372549</v>
@@ -3462,7 +4040,7 @@
         <v>12</v>
       </c>
       <c r="B113" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C113" s="2">
         <v>6.0784313725490193</v>
@@ -3473,7 +4051,7 @@
         <v>12</v>
       </c>
       <c r="B114" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C114" s="2">
         <v>8.764705882352942</v>
@@ -3484,7 +4062,7 @@
         <v>12</v>
       </c>
       <c r="B115" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C115" s="2">
         <v>13.921568627450981</v>
@@ -3495,7 +4073,7 @@
         <v>12</v>
       </c>
       <c r="B116" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C116" s="2">
         <v>8.5882352941176467</v>
@@ -3506,7 +4084,7 @@
         <v>12</v>
       </c>
       <c r="B117" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C117" s="2">
         <v>13.647058823529411</v>
@@ -3517,7 +4095,7 @@
         <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C118" s="2">
         <v>15.196078431372548</v>
@@ -3528,7 +4106,7 @@
         <v>12</v>
       </c>
       <c r="B119" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C119" s="2">
         <v>34.764705882352942</v>
@@ -3539,7 +4117,7 @@
         <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C120" s="2">
         <v>11.607843137254902</v>
@@ -3550,10 +4128,1110 @@
         <v>12</v>
       </c>
       <c r="B121" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C121" s="2">
         <v>11.549019607843137</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>13</v>
+      </c>
+      <c r="B122" t="s">
+        <v>214</v>
+      </c>
+      <c r="C122" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>13</v>
+      </c>
+      <c r="B123" t="s">
+        <v>215</v>
+      </c>
+      <c r="C123" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>13</v>
+      </c>
+      <c r="B124" t="s">
+        <v>216</v>
+      </c>
+      <c r="C124" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>13</v>
+      </c>
+      <c r="B125" t="s">
+        <v>217</v>
+      </c>
+      <c r="C125" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>13</v>
+      </c>
+      <c r="B126" t="s">
+        <v>218</v>
+      </c>
+      <c r="C126" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>13</v>
+      </c>
+      <c r="B127" t="s">
+        <v>219</v>
+      </c>
+      <c r="C127" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>13</v>
+      </c>
+      <c r="B128" t="s">
+        <v>220</v>
+      </c>
+      <c r="C128" s="2">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>13</v>
+      </c>
+      <c r="B129" t="s">
+        <v>221</v>
+      </c>
+      <c r="C129" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>13</v>
+      </c>
+      <c r="B130" t="s">
+        <v>222</v>
+      </c>
+      <c r="C130" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>13</v>
+      </c>
+      <c r="B131" t="s">
+        <v>223</v>
+      </c>
+      <c r="C131" s="2">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>14</v>
+      </c>
+      <c r="B132" t="s">
+        <v>224</v>
+      </c>
+      <c r="C132" s="2">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>14</v>
+      </c>
+      <c r="B133" t="s">
+        <v>225</v>
+      </c>
+      <c r="C133" s="2">
+        <v>57.88</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>14</v>
+      </c>
+      <c r="B134" t="s">
+        <v>226</v>
+      </c>
+      <c r="C134" s="2">
+        <v>70.22</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>14</v>
+      </c>
+      <c r="B135" t="s">
+        <v>227</v>
+      </c>
+      <c r="C135" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>14</v>
+      </c>
+      <c r="B136" t="s">
+        <v>228</v>
+      </c>
+      <c r="C136" s="2">
+        <v>70.11</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>14</v>
+      </c>
+      <c r="B137" t="s">
+        <v>229</v>
+      </c>
+      <c r="C137" s="2">
+        <v>36.54</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>14</v>
+      </c>
+      <c r="B138" t="s">
+        <v>230</v>
+      </c>
+      <c r="C138" s="2">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>14</v>
+      </c>
+      <c r="B139" t="s">
+        <v>231</v>
+      </c>
+      <c r="C139" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>14</v>
+      </c>
+      <c r="B140" t="s">
+        <v>232</v>
+      </c>
+      <c r="C140" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>14</v>
+      </c>
+      <c r="B141" t="s">
+        <v>233</v>
+      </c>
+      <c r="C141" s="2">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>15</v>
+      </c>
+      <c r="B142" t="s">
+        <v>80</v>
+      </c>
+      <c r="C142" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>15</v>
+      </c>
+      <c r="B143" t="s">
+        <v>234</v>
+      </c>
+      <c r="C143" s="2">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>15</v>
+      </c>
+      <c r="B144" t="s">
+        <v>235</v>
+      </c>
+      <c r="C144" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>15</v>
+      </c>
+      <c r="B145" t="s">
+        <v>236</v>
+      </c>
+      <c r="C145" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>15</v>
+      </c>
+      <c r="B146" t="s">
+        <v>237</v>
+      </c>
+      <c r="C146" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>15</v>
+      </c>
+      <c r="B147" t="s">
+        <v>238</v>
+      </c>
+      <c r="C147" s="2">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>15</v>
+      </c>
+      <c r="B148" t="s">
+        <v>239</v>
+      </c>
+      <c r="C148" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>15</v>
+      </c>
+      <c r="B149" t="s">
+        <v>240</v>
+      </c>
+      <c r="C149" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>15</v>
+      </c>
+      <c r="B150" t="s">
+        <v>241</v>
+      </c>
+      <c r="C150" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>15</v>
+      </c>
+      <c r="B151" t="s">
+        <v>242</v>
+      </c>
+      <c r="C151" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>16</v>
+      </c>
+      <c r="B152" t="s">
+        <v>243</v>
+      </c>
+      <c r="C152" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>16</v>
+      </c>
+      <c r="B153" t="s">
+        <v>244</v>
+      </c>
+      <c r="C153" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>16</v>
+      </c>
+      <c r="B154" t="s">
+        <v>245</v>
+      </c>
+      <c r="C154" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>16</v>
+      </c>
+      <c r="B155" t="s">
+        <v>246</v>
+      </c>
+      <c r="C155" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>16</v>
+      </c>
+      <c r="B156" t="s">
+        <v>247</v>
+      </c>
+      <c r="C156" s="2">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>16</v>
+      </c>
+      <c r="B157" t="s">
+        <v>248</v>
+      </c>
+      <c r="C157" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>16</v>
+      </c>
+      <c r="B158" t="s">
+        <v>249</v>
+      </c>
+      <c r="C158" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>16</v>
+      </c>
+      <c r="B159" t="s">
+        <v>250</v>
+      </c>
+      <c r="C159" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>16</v>
+      </c>
+      <c r="B160" t="s">
+        <v>251</v>
+      </c>
+      <c r="C160" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>16</v>
+      </c>
+      <c r="B161" t="s">
+        <v>252</v>
+      </c>
+      <c r="C161" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>22</v>
+      </c>
+      <c r="B162" t="s">
+        <v>83</v>
+      </c>
+      <c r="C162" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>22</v>
+      </c>
+      <c r="B163" t="s">
+        <v>253</v>
+      </c>
+      <c r="C163" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>22</v>
+      </c>
+      <c r="B164" t="s">
+        <v>254</v>
+      </c>
+      <c r="C164" s="2">
+        <v>66.77</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>22</v>
+      </c>
+      <c r="B165" t="s">
+        <v>255</v>
+      </c>
+      <c r="C165" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>22</v>
+      </c>
+      <c r="B166" t="s">
+        <v>256</v>
+      </c>
+      <c r="C166" s="2">
+        <v>23.92</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>22</v>
+      </c>
+      <c r="B167" t="s">
+        <v>257</v>
+      </c>
+      <c r="C167" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>22</v>
+      </c>
+      <c r="B168" t="s">
+        <v>234</v>
+      </c>
+      <c r="C168" s="2">
+        <v>3.37</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>22</v>
+      </c>
+      <c r="B169" t="s">
+        <v>258</v>
+      </c>
+      <c r="C169" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>22</v>
+      </c>
+      <c r="B170" t="s">
+        <v>259</v>
+      </c>
+      <c r="C170" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>22</v>
+      </c>
+      <c r="B171" t="s">
+        <v>260</v>
+      </c>
+      <c r="C171" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>17</v>
+      </c>
+      <c r="B172" t="s">
+        <v>261</v>
+      </c>
+      <c r="C172" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>17</v>
+      </c>
+      <c r="B173" t="s">
+        <v>262</v>
+      </c>
+      <c r="C173" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>17</v>
+      </c>
+      <c r="B174" t="s">
+        <v>78</v>
+      </c>
+      <c r="C174" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>17</v>
+      </c>
+      <c r="B175" t="s">
+        <v>263</v>
+      </c>
+      <c r="C175" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>17</v>
+      </c>
+      <c r="B176" t="s">
+        <v>264</v>
+      </c>
+      <c r="C176" s="2">
+        <v>53.22</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>17</v>
+      </c>
+      <c r="B177" t="s">
+        <v>265</v>
+      </c>
+      <c r="C177" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>17</v>
+      </c>
+      <c r="B178" t="s">
+        <v>266</v>
+      </c>
+      <c r="C178" s="2">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>17</v>
+      </c>
+      <c r="B179" t="s">
+        <v>267</v>
+      </c>
+      <c r="C179" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>17</v>
+      </c>
+      <c r="B180" t="s">
+        <v>268</v>
+      </c>
+      <c r="C180" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>17</v>
+      </c>
+      <c r="B181" t="s">
+        <v>269</v>
+      </c>
+      <c r="C181" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>18</v>
+      </c>
+      <c r="B182" t="s">
+        <v>270</v>
+      </c>
+      <c r="C182" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>18</v>
+      </c>
+      <c r="B183" t="s">
+        <v>271</v>
+      </c>
+      <c r="C183" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>18</v>
+      </c>
+      <c r="B184" t="s">
+        <v>272</v>
+      </c>
+      <c r="C184" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>18</v>
+      </c>
+      <c r="B185" t="s">
+        <v>273</v>
+      </c>
+      <c r="C185" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>18</v>
+      </c>
+      <c r="B186" t="s">
+        <v>265</v>
+      </c>
+      <c r="C186" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>18</v>
+      </c>
+      <c r="B187" t="s">
+        <v>264</v>
+      </c>
+      <c r="C187" s="2">
+        <v>53.22</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>18</v>
+      </c>
+      <c r="B188" t="s">
+        <v>274</v>
+      </c>
+      <c r="C188" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>18</v>
+      </c>
+      <c r="B189" t="s">
+        <v>275</v>
+      </c>
+      <c r="C189" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>18</v>
+      </c>
+      <c r="B190" t="s">
+        <v>276</v>
+      </c>
+      <c r="C190" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>18</v>
+      </c>
+      <c r="B191" t="s">
+        <v>277</v>
+      </c>
+      <c r="C191" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>19</v>
+      </c>
+      <c r="B192" t="s">
+        <v>278</v>
+      </c>
+      <c r="C192" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>19</v>
+      </c>
+      <c r="B193" t="s">
+        <v>279</v>
+      </c>
+      <c r="C193" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>19</v>
+      </c>
+      <c r="B194" t="s">
+        <v>280</v>
+      </c>
+      <c r="C194" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>19</v>
+      </c>
+      <c r="B195" t="s">
+        <v>281</v>
+      </c>
+      <c r="C195" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>19</v>
+      </c>
+      <c r="B196" t="s">
+        <v>282</v>
+      </c>
+      <c r="C196" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>19</v>
+      </c>
+      <c r="B197" t="s">
+        <v>283</v>
+      </c>
+      <c r="C197" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>19</v>
+      </c>
+      <c r="B198" t="s">
+        <v>284</v>
+      </c>
+      <c r="C198" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>19</v>
+      </c>
+      <c r="B199" t="s">
+        <v>285</v>
+      </c>
+      <c r="C199" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>19</v>
+      </c>
+      <c r="B200" t="s">
+        <v>286</v>
+      </c>
+      <c r="C200" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>19</v>
+      </c>
+      <c r="B201" t="s">
+        <v>287</v>
+      </c>
+      <c r="C201" s="2">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>20</v>
+      </c>
+      <c r="B202" t="s">
+        <v>288</v>
+      </c>
+      <c r="C202" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>20</v>
+      </c>
+      <c r="B203" t="s">
+        <v>289</v>
+      </c>
+      <c r="C203" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>20</v>
+      </c>
+      <c r="B204" t="s">
+        <v>290</v>
+      </c>
+      <c r="C204" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>20</v>
+      </c>
+      <c r="B205" t="s">
+        <v>291</v>
+      </c>
+      <c r="C205" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>20</v>
+      </c>
+      <c r="B206" t="s">
+        <v>292</v>
+      </c>
+      <c r="C206" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>20</v>
+      </c>
+      <c r="B207" t="s">
+        <v>293</v>
+      </c>
+      <c r="C207" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>20</v>
+      </c>
+      <c r="B208" t="s">
+        <v>294</v>
+      </c>
+      <c r="C208" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>20</v>
+      </c>
+      <c r="B209" t="s">
+        <v>295</v>
+      </c>
+      <c r="C209" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>20</v>
+      </c>
+      <c r="B210" t="s">
+        <v>296</v>
+      </c>
+      <c r="C210" s="2">
+        <v>47.15</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>20</v>
+      </c>
+      <c r="B211" t="s">
+        <v>297</v>
+      </c>
+      <c r="C211" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>21</v>
+      </c>
+      <c r="B212" t="s">
+        <v>67</v>
+      </c>
+      <c r="C212" s="2">
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>21</v>
+      </c>
+      <c r="B213" t="s">
+        <v>298</v>
+      </c>
+      <c r="C213" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>21</v>
+      </c>
+      <c r="B214" t="s">
+        <v>299</v>
+      </c>
+      <c r="C214" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>21</v>
+      </c>
+      <c r="B215" t="s">
+        <v>300</v>
+      </c>
+      <c r="C215" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>21</v>
+      </c>
+      <c r="B216" t="s">
+        <v>301</v>
+      </c>
+      <c r="C216" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>21</v>
+      </c>
+      <c r="B217" t="s">
+        <v>302</v>
+      </c>
+      <c r="C217" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>21</v>
+      </c>
+      <c r="B218" t="s">
+        <v>303</v>
+      </c>
+      <c r="C218" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>21</v>
+      </c>
+      <c r="B219" t="s">
+        <v>304</v>
+      </c>
+      <c r="C219" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>21</v>
+      </c>
+      <c r="B220" t="s">
+        <v>305</v>
+      </c>
+      <c r="C220" s="2">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>21</v>
+      </c>
+      <c r="B221" t="s">
+        <v>306</v>
+      </c>
+      <c r="C221" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3563,346 +5241,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F981F53D-FAC5-400D-8FEA-1A0C4D8AC9F9}">
-  <dimension ref="A2:P14"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="F2" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="I2" s="10"/>
-      <c r="K2" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="O2" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="P2" s="9"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F4" t="s">
-        <v>167</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" t="s">
-        <v>218</v>
-      </c>
-      <c r="P4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>238</v>
-      </c>
-      <c r="D5" t="s">
-        <v>242</v>
-      </c>
-      <c r="F5" t="s">
-        <v>236</v>
-      </c>
-      <c r="H5" t="s">
-        <v>221</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>431635</v>
-      </c>
-      <c r="L5">
-        <v>300498</v>
-      </c>
-      <c r="M5">
-        <v>114917</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>238</v>
-      </c>
-      <c r="D6" t="s">
-        <v>237</v>
-      </c>
-      <c r="H6" t="s">
-        <v>222</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
-        <v>224</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
-        <v>225</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
-        <v>227</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
-        <v>229</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H12" t="s">
-        <v>231</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H13" t="s">
-        <v>232</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H14" t="s">
-        <v>234</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="H2:I2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="6">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
-    <tablePart r:id="rId6"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EE228D-7BBD-42C8-9A02-CB26DEE7CB0F}">
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C2">
-        <v>1301</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>0.23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3">
-        <v>105282</v>
-      </c>
-      <c r="D3">
-        <v>468</v>
-      </c>
-      <c r="E3">
-        <v>0.44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" t="s">
-        <v>239</v>
-      </c>
-      <c r="C4">
-        <v>1305</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>0.38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C5">
-        <v>54686</v>
-      </c>
-      <c r="D5">
-        <v>248</v>
-      </c>
-      <c r="E5">
-        <v>0.45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>